<commit_message>
feb 6 data updated
</commit_message>
<xml_diff>
--- a/Workbook2.xlsx
+++ b/Workbook2.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t>Male</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>Feb-05</t>
+  </si>
+  <si>
+    <t>Feb-06</t>
+  </si>
+  <si>
+    <t>Mount Elizabeth Novena Hospital, GP Clinic</t>
+  </si>
+  <si>
+    <t>Grand Hyatt Singapore Hotel</t>
   </si>
 </sst>
 </file>
@@ -249,14 +258,14 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -286,11 +295,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,17 +581,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -591,897 +600,982 @@
     <col min="10" max="10" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
         <v>1.2577323</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>103.80979619999999</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="5">
         <v>66</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>1.3075996000000001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>103.8585204</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>53</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>1.257763</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>103.810018</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>37</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>1.2521271512200001</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>103.820006847</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>36</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>1.3081713258200001</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>103.900929093</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>56</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>1.3717759221700001</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>103.944834173</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>56</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>1.28330824331</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>103.860577941</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>35</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>1.350104424</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>103.87764483700001</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>56</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>1.35016073475</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>103.87756705300001</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>56</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>1.2707012</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>103.8631688</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>56</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>1.25210033554</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>103.820199966</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="5">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>1.2521271512200001</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>103.819829822</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="5">
         <v>37</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>1.2854910128799999</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>103.846496344</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="5">
         <v>73</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>1.33608300636</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>103.737467229</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="5">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="5">
         <v>1.3628198948200001</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>103.99087428999999</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="5">
         <v>47</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="I16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>1.2962606000000001</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
         <v>103.8256719</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="5">
         <v>38</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>1.3627072739099999</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>103.991131783</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="5">
         <v>47</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
+      <c r="I18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="5">
         <v>1.3112657863699999</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <v>103.878130317</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="5">
         <v>31</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="5">
         <v>1.2847535909400001</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <v>103.81527811300001</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="5">
         <v>28</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="5">
         <v>1.3747657262399999</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="5">
         <v>103.885970414</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="5">
         <v>48</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="5">
         <v>1.28479917703</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="5">
         <v>103.815087676</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="5">
         <v>44</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="5">
         <v>1.36292983428</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="5">
         <v>103.99122566</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="5">
         <v>41</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="I23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="5">
         <v>1.36307195114</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="5">
         <v>103.99096548599999</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="5">
         <v>17</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="I24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="5">
         <v>1.3793195</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="5">
         <v>103.8826748</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="5">
         <v>32</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="5">
         <v>1.3791659602099999</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="5">
         <v>103.882692754</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="5">
         <v>32</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="5">
         <v>1.3215252096300001</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="5">
         <v>103.847638965</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="5">
         <v>42</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3">
+      <c r="G27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>1.2846570556900001</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="5">
         <v>103.81559461400001</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="5">
         <v>25</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="5">
         <v>1.28469996024</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="5">
         <v>103.815433681</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="5">
         <v>0.6</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="5">
         <v>27</v>
       </c>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1.3222739999999999</v>
+      </c>
+      <c r="C30" s="5">
+        <v>103.84413499999999</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="5">
+        <v>41</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1.3064499999999999</v>
+      </c>
+      <c r="C31" s="5">
+        <v>103.833184</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="5">
+        <v>27</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated on Feb 07
</commit_message>
<xml_diff>
--- a/Workbook2.xlsx
+++ b/Workbook2.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="72">
   <si>
     <t>Male</t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Feb-07</t>
+  </si>
+  <si>
+    <t>Tampines Street 24</t>
+  </si>
+  <si>
+    <t>The Life Church, Missions Singapore</t>
+  </si>
+  <si>
+    <t>Parkway East Hospital</t>
+  </si>
+  <si>
+    <t>Elias Road</t>
+  </si>
+  <si>
+    <t>Sengkang Polyclinic</t>
+  </si>
+  <si>
+    <t>Sengkang</t>
   </si>
 </sst>
 </file>
@@ -584,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1584,6 +1605,99 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
+    <row r="32" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1.3554569999999999</v>
+      </c>
+      <c r="C32" s="5">
+        <v>103.95156299999999</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="5">
+        <v>53</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1.3781049999999999</v>
+      </c>
+      <c r="C33" s="5">
+        <v>103.94172</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="5">
+        <v>42</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1.3926989999999999</v>
+      </c>
+      <c r="C34" s="5">
+        <v>103.894414</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="5">
+        <v>39</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>